<commit_message>
Add proportions to quotes
</commit_message>
<xml_diff>
--- a/data/MisInfoText/Analysis_output/social_media/MisInfoText_social_media_quotes.xlsx
+++ b/data/MisInfoText/Analysis_output/social_media/MisInfoText_social_media_quotes.xlsx
@@ -8,19 +8,25 @@
   </bookViews>
   <sheets>
     <sheet name="2009" sheetId="1" r:id="rId1"/>
-    <sheet name="2013" sheetId="2" r:id="rId2"/>
-    <sheet name="2014" sheetId="3" r:id="rId3"/>
-    <sheet name="2016" sheetId="4" r:id="rId4"/>
-    <sheet name="2017" sheetId="5" r:id="rId5"/>
-    <sheet name="2018" sheetId="6" r:id="rId6"/>
-    <sheet name="Summary" sheetId="7" r:id="rId7"/>
+    <sheet name="2009_proportion" sheetId="2" r:id="rId2"/>
+    <sheet name="2013" sheetId="3" r:id="rId3"/>
+    <sheet name="2013_proportion" sheetId="4" r:id="rId4"/>
+    <sheet name="2014" sheetId="5" r:id="rId5"/>
+    <sheet name="2014_proportion" sheetId="6" r:id="rId6"/>
+    <sheet name="2016" sheetId="7" r:id="rId7"/>
+    <sheet name="2016_proportion" sheetId="8" r:id="rId8"/>
+    <sheet name="2017" sheetId="9" r:id="rId9"/>
+    <sheet name="2017_proportion" sheetId="10" r:id="rId10"/>
+    <sheet name="2018" sheetId="11" r:id="rId11"/>
+    <sheet name="2018_proportion" sheetId="12" r:id="rId12"/>
+    <sheet name="Proportion Summary" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>factcheckURL</t>
   </si>
@@ -28,7 +34,10 @@
     <t>quote</t>
   </si>
   <si>
-    <t>quote_length</t>
+    <t>num_tokens</t>
+  </si>
+  <si>
+    <t>proportion_of_total_tokens</t>
   </si>
   <si>
     <t>http://www.politifact.com/truth-o-meter/statements/2009/aug/13/sarah-palin/palin-claims-obama-misled-when-he-said-end-life-co/</t>
@@ -72,6 +81,9 @@
   </si>
   <si>
     <t>"produces a priority curve on which individuals aged between roughly 15 and 40 years get the most chance, whereas the youngest and oldest people get chances that are attenuated."</t>
+  </si>
+  <si>
+    <t>proportion_quote_tokens_to_total_text</t>
   </si>
   <si>
     <t>http://www.politifact.com/punditfact/statements/2014/jan/06/facebook-posts/facebook-group-no-2-owner-fox-news-prince-alwaleed/</t>
@@ -619,13 +631,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,148 +647,190 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0.03414996288047513</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>0.01484780994803266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>0.005196733481811433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>0.02746844840386043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>0.0155902004454343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>0.008166295471417966</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>0.02375649591685226</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>0.005939123979213066</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>0.006681514476614699</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>0.01930215293244246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>0.005196733481811433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>0.01930215293244246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14">
         <v>33</v>
+      </c>
+      <c r="D14">
+        <v>0.0244988864142539</v>
       </c>
     </row>
   </sheetData>
@@ -799,65 +853,110 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>0.3684210526315789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0.2068965517241379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>0.07045009784735812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>0.1289308176100629</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9">
+        <v>0.4482758620689655</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -867,120 +966,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0.196078431372549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="C3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>0.2166666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4">
         <v>32</v>
       </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>0.5079365079365079</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>0.140625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="C6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>0.3684210526315789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C7">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0.46875</v>
       </c>
     </row>
   </sheetData>
@@ -997,122 +1082,867 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2">
+        <v>0.196078431372549</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>0.2166666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>0.5079365079365079</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>0.140625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>0.3684210526315789</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>0.59375</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1">
+        <v>2009</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.2100965107646622</v>
+      </c>
+      <c r="E2">
+        <v>0.2100965107646622</v>
+      </c>
+      <c r="F2">
+        <v>0.2100965107646622</v>
+      </c>
+      <c r="G2">
+        <v>0.2100965107646622</v>
+      </c>
+      <c r="H2">
+        <v>0.2100965107646622</v>
+      </c>
+      <c r="I2">
+        <v>0.2100965107646622</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1">
+        <v>2013</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0.2094574780058651</v>
+      </c>
+      <c r="D3">
+        <v>0.2512199018790329</v>
+      </c>
+      <c r="E3">
+        <v>0.03181818181818181</v>
+      </c>
+      <c r="F3">
+        <v>0.1206378299120235</v>
+      </c>
+      <c r="G3">
+        <v>0.2094574780058651</v>
+      </c>
+      <c r="H3">
+        <v>0.2982771260997067</v>
+      </c>
+      <c r="I3">
+        <v>0.3870967741935484</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="1">
+        <v>2014</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="E4">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="F4">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="G4">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="H4">
+        <v>0.3846153846153846</v>
+      </c>
+      <c r="I4">
+        <v>0.3846153846153846</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>2016</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0.4742604839858844</v>
+      </c>
+      <c r="D5">
+        <v>0.3336379744232291</v>
+      </c>
+      <c r="E5">
+        <v>0.05494505494505494</v>
+      </c>
+      <c r="F5">
+        <v>0.2456140350877193</v>
+      </c>
+      <c r="G5">
+        <v>0.3478260869565217</v>
+      </c>
+      <c r="H5">
+        <v>0.7545787545787546</v>
+      </c>
+      <c r="I5">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0.286621797735263</v>
+      </c>
+      <c r="D6">
+        <v>0.1505994859465347</v>
+      </c>
+      <c r="E6">
+        <v>0.07045009784735812</v>
+      </c>
+      <c r="F6">
+        <v>0.1874051181956192</v>
+      </c>
+      <c r="G6">
+        <v>0.285</v>
+      </c>
+      <c r="H6">
+        <v>0.3883847549909256</v>
+      </c>
+      <c r="I6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
+        <v>2018</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0.3372462764345505</v>
+      </c>
+      <c r="D7">
+        <v>0.1838634880132777</v>
+      </c>
+      <c r="E7">
+        <v>0.140625</v>
+      </c>
+      <c r="F7">
+        <v>0.2012254901960784</v>
+      </c>
+      <c r="G7">
+        <v>0.2925438596491228</v>
+      </c>
+      <c r="H7">
+        <v>0.4730576441102757</v>
+      </c>
+      <c r="I7">
+        <v>0.59375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0.2100965107646622</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.3870967741935484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>0.03181818181818181</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>0.3870967741935484</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>0.03181818181818181</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0.3846153846153846</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>0.3846153846153846</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>0.1578947368421053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0.05494505494505494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5">
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>0.7948717948717948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
         <v>37</v>
       </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>0.3478260869565217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>0.1578947368421053</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>0.05494505494505494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>0.7948717948717948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>0.9166666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>0.3478260869565217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>0.3684210526315789</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>0.2068965517241379</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>0.07045009784735812</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>0.07547169811320754</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>0.05345911949685535</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>13</v>
+      </c>
+      <c r="D10">
+        <v>0.4482758620689655</v>
       </c>
     </row>
   </sheetData>
@@ -1129,327 +1959,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1">
-        <v>2009</v>
-      </c>
-      <c r="B2">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>21.76923076923077</v>
-      </c>
-      <c r="D2">
-        <v>12.89155955237021</v>
-      </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>9</v>
-      </c>
-      <c r="G2">
-        <v>21</v>
-      </c>
-      <c r="H2">
-        <v>32</v>
-      </c>
-      <c r="I2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="1">
-        <v>2013</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>9.5</v>
-      </c>
-      <c r="D3">
-        <v>3.535533905932738</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>8.25</v>
-      </c>
-      <c r="G3">
-        <v>9.5</v>
-      </c>
-      <c r="H3">
-        <v>10.75</v>
-      </c>
-      <c r="I3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>2014</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>2016</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>16.85714285714286</v>
-      </c>
-      <c r="D5">
-        <v>9.026416258748013</v>
-      </c>
-      <c r="E5">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>23.5</v>
-      </c>
-      <c r="I5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
-        <v>2017</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>17.88888888888889</v>
-      </c>
-      <c r="D6">
-        <v>21.16863507907657</v>
-      </c>
-      <c r="E6">
-        <v>6</v>
-      </c>
-      <c r="F6">
-        <v>7</v>
-      </c>
-      <c r="G6">
-        <v>8</v>
-      </c>
-      <c r="H6">
-        <v>17</v>
-      </c>
-      <c r="I6">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
-        <v>2018</v>
-      </c>
-      <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>16.57142857142857</v>
-      </c>
-      <c r="D7">
-        <v>10.09714716899684</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>9.5</v>
-      </c>
-      <c r="G7">
-        <v>13</v>
-      </c>
-      <c r="H7">
-        <v>22</v>
-      </c>
-      <c r="I7">
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Apply is_word check to quotes
</commit_message>
<xml_diff>
--- a/data/MisInfoText/Analysis_output/social_media/MisInfoText_social_media_quotes.xlsx
+++ b/data/MisInfoText/Analysis_output/social_media/MisInfoText_social_media_quotes.xlsx
@@ -34,10 +34,10 @@
     <t>quote</t>
   </si>
   <si>
-    <t>num_tokens</t>
-  </si>
-  <si>
-    <t>proportion_of_total_tokens</t>
+    <t>num_words</t>
+  </si>
+  <si>
+    <t>proportion_of_total_words</t>
   </si>
   <si>
     <t>http://www.politifact.com/truth-o-meter/statements/2009/aug/13/sarah-palin/palin-claims-obama-misled-when-he-said-end-life-co/</t>
@@ -83,7 +83,7 @@
     <t>"produces a priority curve on which individuals aged between roughly 15 and 40 years get the most chance, whereas the youngest and oldest people get chances that are attenuated."</t>
   </si>
   <si>
-    <t>proportion_quote_tokens_to_total_text</t>
+    <t>proportion_quote_words_to_total_words</t>
   </si>
   <si>
     <t>http://www.politifact.com/punditfact/statements/2014/jan/06/facebook-posts/facebook-group-no-2-owner-fox-news-prince-alwaleed/</t>
@@ -659,10 +659,10 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D2">
-        <v>0.03414996288047513</v>
+        <v>0.0368968779564806</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -673,10 +673,10 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>0.01484780994803266</v>
+        <v>0.01797540208136235</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -687,10 +687,10 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>0.005196733481811433</v>
+        <v>0.003784295175023652</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -701,10 +701,10 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <v>0.02746844840386043</v>
+        <v>0.02838221381267739</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -715,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>0.0155902004454343</v>
+        <v>0.0141911069063387</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -729,10 +729,10 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D7">
-        <v>0.008166295471417966</v>
+        <v>0.007568590350047304</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -743,10 +743,10 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8">
-        <v>0.02375649591685226</v>
+        <v>0.02554399243140965</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -757,10 +757,10 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0.005939123979213066</v>
+        <v>0.003784295175023652</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -771,10 +771,10 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D10">
-        <v>0.006681514476614699</v>
+        <v>0.005676442762535478</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -785,10 +785,10 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>0.01930215293244246</v>
+        <v>0.01986754966887417</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -799,10 +799,10 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>0.005196733481811433</v>
+        <v>0.004730368968779565</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -813,10 +813,10 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D13">
-        <v>0.01930215293244246</v>
+        <v>0.02081362346263009</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -827,10 +827,10 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D14">
-        <v>0.0244988864142539</v>
+        <v>0.02743614001892148</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +874,7 @@
         <v>39</v>
       </c>
       <c r="B2">
-        <v>0.3684210526315789</v>
+        <v>0.3076923076923077</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -882,7 +882,7 @@
         <v>40</v>
       </c>
       <c r="B3">
-        <v>0.2068965517241379</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -890,7 +890,7 @@
         <v>41</v>
       </c>
       <c r="B4">
-        <v>0.07045009784735812</v>
+        <v>0.07331042382588775</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -898,7 +898,7 @@
         <v>42</v>
       </c>
       <c r="B5">
-        <v>0.32</v>
+        <v>0.3181818181818182</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -906,7 +906,7 @@
         <v>43</v>
       </c>
       <c r="B6">
-        <v>0.1289308176100629</v>
+        <v>0.1439688715953307</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -914,7 +914,7 @@
         <v>44</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.5384615384615384</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -922,7 +922,7 @@
         <v>45</v>
       </c>
       <c r="B8">
-        <v>0.25</v>
+        <v>0.1739130434782609</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -930,7 +930,7 @@
         <v>46</v>
       </c>
       <c r="B9">
-        <v>0.4482758620689655</v>
+        <v>0.4814814814814815</v>
       </c>
     </row>
   </sheetData>
@@ -981,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>0.196078431372549</v>
+        <v>0.2325581395348837</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -995,7 +995,7 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>0.2166666666666667</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1006,10 +1006,10 @@
         <v>64</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D4">
-        <v>0.5079365079365079</v>
+        <v>0.5094339622641509</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1020,10 +1020,10 @@
         <v>65</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>0.140625</v>
+        <v>0.1509433962264151</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1034,10 +1034,10 @@
         <v>66</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>0.3684210526315789</v>
+        <v>0.3870967741935484</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1048,10 +1048,10 @@
         <v>67</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7">
-        <v>0.125</v>
+        <v>0.1041666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1062,10 +1062,10 @@
         <v>68</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>0.46875</v>
+        <v>0.5208333333333334</v>
       </c>
     </row>
   </sheetData>
@@ -1103,7 +1103,7 @@
         <v>56</v>
       </c>
       <c r="B2">
-        <v>0.196078431372549</v>
+        <v>0.2325581395348837</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1111,7 +1111,7 @@
         <v>57</v>
       </c>
       <c r="B3">
-        <v>0.2166666666666667</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1119,7 +1119,7 @@
         <v>58</v>
       </c>
       <c r="B4">
-        <v>0.5079365079365079</v>
+        <v>0.5094339622641509</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1127,7 +1127,7 @@
         <v>59</v>
       </c>
       <c r="B5">
-        <v>0.140625</v>
+        <v>0.1509433962264151</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1135,7 +1135,7 @@
         <v>60</v>
       </c>
       <c r="B6">
-        <v>0.3684210526315789</v>
+        <v>0.3870967741935484</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1143,7 +1143,7 @@
         <v>61</v>
       </c>
       <c r="B7">
-        <v>0.59375</v>
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>
@@ -1204,22 +1204,22 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
       <c r="E2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
       <c r="F2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
       <c r="G2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
       <c r="H2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
       <c r="I2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1230,25 +1230,25 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>0.2094574780058651</v>
+        <v>0.2032894736842105</v>
       </c>
       <c r="D3">
-        <v>0.2512199018790329</v>
+        <v>0.2428353551180117</v>
       </c>
       <c r="E3">
-        <v>0.03181818181818181</v>
+        <v>0.03157894736842105</v>
       </c>
       <c r="F3">
-        <v>0.1206378299120235</v>
+        <v>0.1174342105263158</v>
       </c>
       <c r="G3">
-        <v>0.2094574780058651</v>
+        <v>0.2032894736842105</v>
       </c>
       <c r="H3">
-        <v>0.2982771260997067</v>
+        <v>0.2891447368421053</v>
       </c>
       <c r="I3">
-        <v>0.3870967741935484</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1259,22 +1259,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
       <c r="E4">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
       <c r="F4">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
       <c r="G4">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
       <c r="H4">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
       <c r="I4">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1285,25 +1285,25 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>0.4742604839858844</v>
+        <v>0.5130284573281968</v>
       </c>
       <c r="D5">
-        <v>0.3336379744232291</v>
+        <v>0.3353992533178889</v>
       </c>
       <c r="E5">
-        <v>0.05494505494505494</v>
+        <v>0.06211180124223602</v>
       </c>
       <c r="F5">
-        <v>0.2456140350877193</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G5">
-        <v>0.3478260869565217</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="H5">
-        <v>0.7545787545787546</v>
+        <v>0.8200992555831266</v>
       </c>
       <c r="I5">
-        <v>0.9166666666666666</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1314,25 +1314,25 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.286621797735263</v>
+        <v>0.2858761855895782</v>
       </c>
       <c r="D6">
-        <v>0.1505994859465347</v>
+        <v>0.1615660519815501</v>
       </c>
       <c r="E6">
-        <v>0.07045009784735812</v>
+        <v>0.07331042382588775</v>
       </c>
       <c r="F6">
-        <v>0.1874051181956192</v>
+        <v>0.1664270005075283</v>
       </c>
       <c r="G6">
-        <v>0.285</v>
+        <v>0.2788461538461539</v>
       </c>
       <c r="H6">
-        <v>0.3883847549909256</v>
+        <v>0.359006734006734</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>0.5384615384615384</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1343,25 +1343,25 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.3372462764345505</v>
+        <v>0.3608387120364997</v>
       </c>
       <c r="D7">
-        <v>0.1838634880132777</v>
+        <v>0.18068293500081</v>
       </c>
       <c r="E7">
-        <v>0.140625</v>
+        <v>0.1509433962264151</v>
       </c>
       <c r="F7">
-        <v>0.2012254901960784</v>
+        <v>0.2394186046511628</v>
       </c>
       <c r="G7">
-        <v>0.2925438596491228</v>
+        <v>0.3235483870967742</v>
       </c>
       <c r="H7">
-        <v>0.4730576441102757</v>
+        <v>0.4788496652465003</v>
       </c>
       <c r="I7">
-        <v>0.59375</v>
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>
@@ -1390,7 +1390,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.2100965107646622</v>
+        <v>0.216650898770104</v>
       </c>
     </row>
   </sheetData>
@@ -1431,10 +1431,10 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D2">
-        <v>0.3870967741935484</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1445,10 +1445,10 @@
         <v>22</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>0.03181818181818181</v>
+        <v>0.03157894736842105</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1481,7 @@
         <v>19</v>
       </c>
       <c r="B2">
-        <v>0.3870967741935484</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1489,7 +1489,7 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <v>0.03181818181818181</v>
+        <v>0.03157894736842105</v>
       </c>
     </row>
   </sheetData>
@@ -1531,10 +1531,10 @@
         <v>24</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="B2">
-        <v>0.3846153846153846</v>
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>
@@ -1610,7 +1610,7 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>0.1578947368421053</v>
+        <v>0.1714285714285714</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1624,7 +1624,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>0.05494505494505494</v>
+        <v>0.06211180124223602</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1635,10 +1635,10 @@
         <v>34</v>
       </c>
       <c r="C4">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>0.7142857142857143</v>
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1649,10 +1649,10 @@
         <v>35</v>
       </c>
       <c r="C5">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>0.7948717948717948</v>
+        <v>0.8709677419354839</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1663,10 +1663,10 @@
         <v>36</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>0.9166666666666666</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1680,7 +1680,7 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>0.3478260869565217</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1691,10 +1691,10 @@
         <v>38</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8">
-        <v>0.3333333333333333</v>
+        <v>0.4285714285714285</v>
       </c>
     </row>
   </sheetData>
@@ -1732,7 +1732,7 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>0.1578947368421053</v>
+        <v>0.1714285714285714</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1740,7 +1740,7 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>0.05494505494505494</v>
+        <v>0.06211180124223602</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1748,7 +1748,7 @@
         <v>27</v>
       </c>
       <c r="B4">
-        <v>0.7142857142857143</v>
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1756,7 +1756,7 @@
         <v>28</v>
       </c>
       <c r="B5">
-        <v>0.7948717948717948</v>
+        <v>0.8709677419354839</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1764,7 +1764,7 @@
         <v>29</v>
       </c>
       <c r="B6">
-        <v>0.9166666666666666</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1772,7 +1772,7 @@
         <v>30</v>
       </c>
       <c r="B7">
-        <v>0.3478260869565217</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1780,7 +1780,7 @@
         <v>31</v>
       </c>
       <c r="B8">
-        <v>0.3333333333333333</v>
+        <v>0.4285714285714285</v>
       </c>
     </row>
   </sheetData>
@@ -1827,10 +1827,10 @@
         <v>47</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>0.3684210526315789</v>
+        <v>0.3076923076923077</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1844,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>0.2068965517241379</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1855,10 +1855,10 @@
         <v>49</v>
       </c>
       <c r="C4">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D4">
-        <v>0.07045009784735812</v>
+        <v>0.07331042382588775</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1869,10 +1869,10 @@
         <v>50</v>
       </c>
       <c r="C5">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>0.32</v>
+        <v>0.3181818181818182</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1883,10 +1883,10 @@
         <v>51</v>
       </c>
       <c r="C6">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6">
-        <v>0.07547169811320754</v>
+        <v>0.08560311284046693</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1897,10 +1897,10 @@
         <v>52</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>0.05345911949685535</v>
+        <v>0.05836575875486381</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1914,7 +1914,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.5384615384615384</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1925,10 +1925,10 @@
         <v>54</v>
       </c>
       <c r="C9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D9">
-        <v>0.25</v>
+        <v>0.1739130434782609</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1942,7 +1942,7 @@
         <v>13</v>
       </c>
       <c r="D10">
-        <v>0.4482758620689655</v>
+        <v>0.4814814814814815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>